<commit_message>
this is update for radio
</commit_message>
<xml_diff>
--- a/updatelist_kaigai.xlsx
+++ b/updatelist_kaigai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narawanozomi/Documents/4pro/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAB73BA-F106-C24E-8E39-44BDF2612E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C1033D-B5B9-5A43-BEE6-F46887E487FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="197">
   <si>
     <t>問題</t>
   </si>
@@ -1467,13 +1467,88 @@
       </rPr>
       <t>通行人に道を尋ねて案内してもらう</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>選択肢</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">センタクシ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>選択肢</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">センタクシ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="MS Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>選択肢</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">センタクシ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1517,6 +1592,19 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1538,7 +1626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1550,6 +1638,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1770,8 +1859,8 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1790,6 +1879,15 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2">

</xml_diff>